<commit_message>
Oppdatert større næring for levering til nettet ++
</commit_message>
<xml_diff>
--- a/Prissatser_nettleie_Glitre.xlsx
+++ b/Prissatser_nettleie_Glitre.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asmund.fossum\Documents\Strømpriser\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\asmund.fossum\Documents\Strompriser\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F2520078-C3A6-4AA4-A194-76648723C265}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F80F5897-3515-443D-BCC3-8FB04349DCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-23148" yWindow="3492" windowWidth="23256" windowHeight="12576" xr2:uid="{846E382B-0241-4CBD-8E39-0843AEB05BE3}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="30936" windowHeight="16776" activeTab="2" xr2:uid="{846E382B-0241-4CBD-8E39-0843AEB05BE3}"/>
   </bookViews>
   <sheets>
     <sheet name="Privatkunde" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="77" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="49">
   <si>
     <t>Kapasitetsledd</t>
   </si>
@@ -176,6 +176,15 @@
   </si>
   <si>
     <t>Inkl. mva. (kr/mnd)</t>
+  </si>
+  <si>
+    <t>Energiledd sommer</t>
+  </si>
+  <si>
+    <t>Energiledd vinter</t>
+  </si>
+  <si>
+    <t>Oppdatert</t>
   </si>
 </sst>
 </file>
@@ -260,7 +269,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -307,6 +316,9 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -327,9 +339,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-tema">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013–2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -367,7 +379,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013–2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -473,7 +485,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013–2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -615,7 +627,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -625,25 +637,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{711BC047-462D-4916-A1EB-232D01805D89}">
   <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="23.7109375" customWidth="1"/>
+    <col min="1" max="1" width="23.6640625" customWidth="1"/>
     <col min="2" max="3" width="21" customWidth="1"/>
-    <col min="4" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="23.140625" customWidth="1"/>
-    <col min="6" max="6" width="23.7109375" customWidth="1"/>
-    <col min="7" max="7" width="37.28515625" customWidth="1"/>
+    <col min="4" max="4" width="20.6640625" customWidth="1"/>
+    <col min="5" max="5" width="23.109375" customWidth="1"/>
+    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="7" max="7" width="37.33203125" customWidth="1"/>
     <col min="8" max="8" width="34" customWidth="1"/>
     <col min="9" max="9" width="5" customWidth="1"/>
-    <col min="10" max="10" width="22.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.85546875" customWidth="1"/>
+    <col min="10" max="10" width="22.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -675,7 +687,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -709,7 +721,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -743,7 +755,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -777,7 +789,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -798,7 +810,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -817,7 +829,7 @@
       </c>
       <c r="F6" s="4"/>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -835,7 +847,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -853,7 +865,7 @@
         <v>1216</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -871,7 +883,7 @@
         <v>1920</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -889,7 +901,7 @@
         <v>2560</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -921,22 +933,22 @@
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="23" customWidth="1"/>
-    <col min="2" max="2" width="21.140625" customWidth="1"/>
+    <col min="2" max="2" width="21.109375" customWidth="1"/>
     <col min="3" max="3" width="20" customWidth="1"/>
-    <col min="4" max="4" width="22.140625" customWidth="1"/>
-    <col min="5" max="5" width="34.5703125" customWidth="1"/>
-    <col min="6" max="6" width="22.7109375" customWidth="1"/>
+    <col min="4" max="4" width="22.109375" customWidth="1"/>
+    <col min="5" max="5" width="34.5546875" customWidth="1"/>
+    <col min="6" max="6" width="22.6640625" customWidth="1"/>
     <col min="7" max="7" width="36" customWidth="1"/>
-    <col min="8" max="8" width="32.5703125" customWidth="1"/>
-    <col min="9" max="9" width="2.85546875" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="32.5546875" customWidth="1"/>
+    <col min="9" max="9" width="2.88671875" customWidth="1"/>
+    <col min="10" max="10" width="24.6640625" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -968,7 +980,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1002,7 +1014,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>2</v>
       </c>
@@ -1036,7 +1048,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A4" s="2" t="s">
         <v>3</v>
       </c>
@@ -1070,7 +1082,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>4</v>
       </c>
@@ -1091,7 +1103,7 @@
       <c r="G5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A6" s="2" t="s">
         <v>5</v>
       </c>
@@ -1109,7 +1121,7 @@
         <v>690.67</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A7" s="2" t="s">
         <v>6</v>
       </c>
@@ -1127,7 +1139,7 @@
         <v>850.67</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
         <v>7</v>
       </c>
@@ -1145,7 +1157,7 @@
         <v>1282.67</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
         <v>8</v>
       </c>
@@ -1163,7 +1175,7 @@
         <v>1986.67</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
         <v>9</v>
       </c>
@@ -1181,7 +1193,7 @@
         <v>2626.67</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
         <v>10</v>
       </c>
@@ -1206,26 +1218,26 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0DB0D84-46A6-47E1-B7A1-73857261DBF1}">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:E13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" customWidth="1"/>
-    <col min="2" max="2" width="25.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.140625" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" customWidth="1"/>
-    <col min="5" max="5" width="60.42578125" customWidth="1"/>
-    <col min="6" max="6" width="34.7109375" customWidth="1"/>
-    <col min="7" max="7" width="26.5703125" customWidth="1"/>
-    <col min="8" max="8" width="27.5703125" customWidth="1"/>
-    <col min="9" max="9" width="20.7109375" customWidth="1"/>
+    <col min="1" max="1" width="36.44140625" customWidth="1"/>
+    <col min="2" max="2" width="25.88671875" customWidth="1"/>
+    <col min="3" max="3" width="27.109375" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" customWidth="1"/>
+    <col min="5" max="5" width="22.109375" customWidth="1"/>
+    <col min="6" max="6" width="34.6640625" customWidth="1"/>
+    <col min="7" max="7" width="26.5546875" customWidth="1"/>
+    <col min="8" max="8" width="27.5546875" customWidth="1"/>
+    <col min="9" max="9" width="20.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>26</v>
       </c>
@@ -1238,160 +1250,186 @@
       <c r="D1" s="10" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E1" s="10" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>27</v>
       </c>
       <c r="B2" s="11">
+        <f>B3*12</f>
         <v>6000</v>
       </c>
       <c r="C2" s="11">
-        <v>6000</v>
+        <f>C3*12</f>
+        <v>12000</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>28</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
+      <c r="E2" s="18">
+        <v>45575</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A3" s="16"/>
       <c r="B3" s="7">
         <v>500</v>
       </c>
       <c r="C3" s="7">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B4" s="9">
-        <v>5.5</v>
-      </c>
-      <c r="C4" s="9">
-        <v>4.2</v>
-      </c>
-      <c r="D4" s="8" t="s">
+    <row r="4" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A4" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="7">
+        <v>7.9</v>
+      </c>
+      <c r="C4" s="7">
+        <v>6.6</v>
+      </c>
+      <c r="D4" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A5" s="16" t="s">
+    <row r="5" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A5" s="8" t="s">
+        <v>47</v>
+      </c>
+      <c r="B5" s="9">
+        <v>7.9</v>
+      </c>
+      <c r="C5" s="9">
+        <v>6.6</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A6" s="16" t="s">
         <v>31</v>
       </c>
-      <c r="B5" s="11">
-        <v>1080</v>
-      </c>
-      <c r="C5" s="7">
-        <v>936</v>
-      </c>
-      <c r="D5" s="6" t="s">
+      <c r="B6" s="11">
+        <f>B7*12</f>
+        <v>1296</v>
+      </c>
+      <c r="C6" s="11">
+        <f>C7*12</f>
+        <v>1152</v>
+      </c>
+      <c r="D6" s="6" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A6" s="16"/>
-      <c r="B6" s="7">
-        <v>90</v>
-      </c>
-      <c r="C6" s="7">
-        <v>78</v>
-      </c>
-      <c r="D6" s="6" t="s">
+    <row r="7" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A7" s="16"/>
+      <c r="B7" s="7">
+        <v>108</v>
+      </c>
+      <c r="C7" s="7">
+        <v>96</v>
+      </c>
+      <c r="D7" s="6" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A7" s="17" t="s">
+    <row r="8" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A8" s="17" t="s">
         <v>34</v>
       </c>
-      <c r="B7" s="9">
-        <v>360</v>
-      </c>
-      <c r="C7" s="9">
-        <v>300</v>
-      </c>
-      <c r="D7" s="8" t="s">
+      <c r="B8" s="9">
+        <f>B9*12</f>
+        <v>432</v>
+      </c>
+      <c r="C8" s="9">
+        <f>C9*12</f>
+        <v>384</v>
+      </c>
+      <c r="D8" s="8" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A8" s="17"/>
-      <c r="B8" s="9">
+    <row r="9" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="9">
+        <v>36</v>
+      </c>
+      <c r="C9" s="9">
+        <v>32</v>
+      </c>
+      <c r="D9" s="8" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A10" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="7">
+        <v>9.51</v>
+      </c>
+      <c r="C10" s="7">
+        <v>9.51</v>
+      </c>
+      <c r="D10" s="6" t="s">
         <v>30</v>
       </c>
-      <c r="C8" s="9">
-        <v>25</v>
-      </c>
-      <c r="D8" s="8" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A9" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="B9" s="7">
-        <v>9.16</v>
-      </c>
-      <c r="C9" s="7">
-        <v>9.16</v>
-      </c>
-      <c r="D9" s="6" t="s">
+    </row>
+    <row r="11" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A11" s="8" t="s">
+        <v>36</v>
+      </c>
+      <c r="B11" s="9">
+        <v>16.440000000000001</v>
+      </c>
+      <c r="C11" s="9">
+        <v>16.440000000000001</v>
+      </c>
+      <c r="D11" s="8" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A10" s="8" t="s">
-        <v>36</v>
-      </c>
-      <c r="B10" s="9">
-        <v>15.84</v>
-      </c>
-      <c r="C10" s="9">
-        <v>15.84</v>
-      </c>
-      <c r="D10" s="8" t="s">
+    <row r="12" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A12" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="B12" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C12" s="7">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D12" s="6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A11" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B11" s="7">
-        <v>0.54600000000000004</v>
-      </c>
-      <c r="C11" s="7">
-        <v>0.54600000000000004</v>
-      </c>
-      <c r="D11" s="6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
+    <row r="13" spans="1:5" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A13" s="8" t="s">
         <v>38</v>
       </c>
-      <c r="B12" s="9">
+      <c r="B13" s="9">
         <v>800</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C13" s="9">
         <v>800</v>
       </c>
-      <c r="D12" s="8" t="s">
+      <c r="D13" s="8" t="s">
         <v>28</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="3">
     <mergeCell ref="A2:A3"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="A7:A8"/>
+    <mergeCell ref="A6:A7"/>
+    <mergeCell ref="A8:A9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>

</xml_diff>